<commit_message>
rev 5 normal mode completed. not standalone yet.
</commit_message>
<xml_diff>
--- a/hardware/rev 5/Aries parts list rev 5.xlsx
+++ b/hardware/rev 5/Aries parts list rev 5.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{FE589F85-F430-46E0-9844-581DB2745167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B02F053C-5495-487A-ACD1-958CA7D52CB7}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{FE589F85-F430-46E0-9844-581DB2745167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3BCB396A-8E9D-4196-9733-7F0E99F1B940}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="1755" windowWidth="19125" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Embedded ATU" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="189">
   <si>
     <t>RL1-RL17</t>
   </si>
@@ -425,9 +425,6 @@
     <t>5T 18 SWG</t>
   </si>
   <si>
-    <t>Wiring Modifications</t>
-  </si>
-  <si>
     <t>20pF mica</t>
   </si>
   <si>
@@ -470,9 +467,6 @@
     <t>primary: 1T 22 SWG through centre</t>
   </si>
   <si>
-    <t>The VSWR bridge is now a binocular core using a BN-61-202 core</t>
-  </si>
-  <si>
     <t>BNC rt angle</t>
   </si>
   <si>
@@ -485,9 +479,6 @@
     <t>L22</t>
   </si>
   <si>
-    <t>wire jumper 1-2</t>
-  </si>
-  <si>
     <t>R1, R2, R41-R44</t>
   </si>
   <si>
@@ -552,9 +543,6 @@
   </si>
   <si>
     <t>header 4 pin 0.1" pitch</t>
-  </si>
-  <si>
-    <t>J5, J6, 17</t>
   </si>
   <si>
     <t>J19</t>
@@ -584,6 +572,33 @@
   </si>
   <si>
     <t>secondary: 14T 26 SWG wound around the sides of the core</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>SMA-SMA</t>
+  </si>
+  <si>
+    <t>J2-J3</t>
+  </si>
+  <si>
+    <t>J5, J6, J17</t>
+  </si>
+  <si>
+    <t>SK17</t>
+  </si>
+  <si>
+    <t>add a jumper on SK17 for "standalone" ATU mode</t>
+  </si>
+  <si>
+    <t>The VSWR bridge is now a binocular core using a BN-61-202 core, 14 turns</t>
+  </si>
+  <si>
+    <t>wire</t>
+  </si>
+  <si>
+    <t>jumper pin 1-2</t>
   </si>
 </sst>
 </file>
@@ -699,23 +714,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ABCE919-228F-410E-BEB6-69DCF5D8FB6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4583247C-8A2C-472D-A09C-B56CAEEC335F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -737,7 +752,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="114300" y="13858875"/>
+          <a:off x="438150" y="16440150"/>
           <a:ext cx="2743200" cy="1419225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1071,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
@@ -1197,16 +1212,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1248,10 +1263,10 @@
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>16</v>
@@ -1317,7 +1332,7 @@
         <v>52</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>21</v>
@@ -1339,7 +1354,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1387,7 +1402,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1435,7 +1450,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1451,7 +1466,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1477,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>21</v>
@@ -1506,10 +1521,10 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>21</v>
@@ -1525,7 +1540,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>21</v>
@@ -1541,16 +1556,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1575,7 +1590,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>37</v>
@@ -1629,7 +1644,7 @@
         <v>37</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1647,7 +1662,7 @@
         <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1682,10 +1697,10 @@
         <v>92</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="10"/>
@@ -1696,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>83</v>
@@ -1734,7 +1749,7 @@
         <v>83</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1762,13 +1777,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1796,16 +1811,16 @@
         <v>2</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -1882,13 +1897,13 @@
         <v>2</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1898,13 +1913,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -1914,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>95</v>
@@ -1928,129 +1943,143 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="5">
+        <v>1</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>106</v>
-      </c>
-      <c r="B54" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C56" t="s">
-        <v>139</v>
+        <v>107</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C61" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B64" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C64" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>151</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>147</v>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+    </row>
+    <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>184</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2065,14 +2094,14 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
   </cols>
@@ -2100,7 +2129,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2148,10 +2177,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2165,11 +2194,11 @@
         <v>69</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -2258,7 +2287,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1</v>
@@ -2276,7 +2305,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -2288,7 +2317,20 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+      <c r="A14" s="5">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>